<commit_message>
organized silk screen and swd tp
</commit_message>
<xml_diff>
--- a/pcb/draft_1-2/BOM.xlsx
+++ b/pcb/draft_1-2/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\EletronicEgg\pcb\draft_1-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B2A73E0-13CB-4AF1-B1BE-16C86FD0AEF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F976B4E-3F08-4477-8CBA-34B24CCE59FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CC748F4A-B77A-42D3-919B-40EFF9144FCF}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t>400 mAh Battery</t>
   </si>
@@ -259,6 +259,12 @@
   </si>
   <si>
     <t>Flux</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/vishay-semiconductor-opto-division/TLMS1000-GS08/TLMS1000-GS08CT-ND/4743829</t>
+  </si>
+  <si>
+    <t>Red LED 0603, 2mA 1.8V</t>
   </si>
 </sst>
 </file>
@@ -1798,7 +1804,7 @@
   <dimension ref="A1:AM48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3975,6 +3981,14 @@
         <v>75</v>
       </c>
     </row>
+    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>77</v>
+      </c>
+      <c r="E26" t="s">
+        <v>76</v>
+      </c>
+    </row>
     <row r="28" spans="1:39" x14ac:dyDescent="0.25">
       <c r="X28">
         <v>1</v>

</xml_diff>

<commit_message>
pngs and bob as-ordered
</commit_message>
<xml_diff>
--- a/pcb/draft_1-2/BOM.xlsx
+++ b/pcb/draft_1-2/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\EletronicEgg\pcb\draft_1-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C61987D-AFD5-4762-8A45-4445BB9427E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F313FFCC-8FF0-4509-8BFF-44091B770F0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="3435" windowWidth="21600" windowHeight="11385" xr2:uid="{CC748F4A-B77A-42D3-919B-40EFF9144FCF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CC748F4A-B77A-42D3-919B-40EFF9144FCF}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
   <si>
     <t>400 mAh Battery</t>
   </si>
@@ -325,6 +325,15 @@
   </si>
   <si>
     <t>08055C104KAT4A</t>
+  </si>
+  <si>
+    <t>TLMS1000-GS08</t>
+  </si>
+  <si>
+    <t>100 mil headers, male</t>
+  </si>
+  <si>
+    <t>J2</t>
   </si>
 </sst>
 </file>
@@ -351,7 +360,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -370,6 +379,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -383,7 +398,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -396,6 +411,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1857,14 +1873,14 @@
   <dimension ref="A1:AN50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="114" bestFit="1" customWidth="1"/>
@@ -1878,7 +1894,7 @@
         <v>51</v>
       </c>
       <c r="B1" s="5">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="C1" s="5"/>
       <c r="K1" t="s">
@@ -1897,7 +1913,7 @@
       </c>
       <c r="B2" s="8">
         <f>AN26</f>
-        <v>107.1</v>
+        <v>36.783299999999997</v>
       </c>
       <c r="C2" s="8"/>
     </row>
@@ -2035,7 +2051,7 @@
       </c>
       <c r="E5" s="6">
         <f t="shared" ref="E5:E25" si="4">_xlfn.MAXIFS(AF$4:AM$4,AF5:AM5,CONCATENATE("=",AN5))</f>
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>5</v>
@@ -2048,7 +2064,7 @@
       </c>
       <c r="V5">
         <f t="shared" ref="V5:V25" si="5">B$1*D5</f>
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="W5">
         <f t="shared" ref="W5:W25" si="6">K5</f>
@@ -2088,31 +2104,31 @@
       </c>
       <c r="AG5">
         <f t="shared" ref="AG5:AG25" si="15">X5*MAX($V5,AG$4)/$B$1</f>
-        <v>12.375</v>
+        <v>4.95</v>
       </c>
       <c r="AH5">
         <f t="shared" ref="AH5:AH25" si="16">Y5*MAX($V5,AH$4)/$B$1</f>
-        <v>24.75</v>
+        <v>4.95</v>
       </c>
       <c r="AI5">
         <f t="shared" ref="AI5:AI25" si="17">Z5*MAX($V5,AI$4)/$B$1</f>
-        <v>61.875</v>
+        <v>4.95</v>
       </c>
       <c r="AJ5">
         <f t="shared" ref="AJ5:AJ25" si="18">AA5*MAX($V5,AJ$4)/$B$1</f>
-        <v>123.75</v>
+        <v>9.9</v>
       </c>
       <c r="AK5">
         <f t="shared" ref="AK5:AK25" si="19">AB5*MAX($V5,AK$4)/$B$1</f>
-        <v>247.5</v>
+        <v>19.8</v>
       </c>
       <c r="AL5">
         <f t="shared" ref="AL5:AL25" si="20">AC5*MAX($V5,AL$4)/$B$1</f>
-        <v>1237.5</v>
+        <v>99</v>
       </c>
       <c r="AM5">
         <f t="shared" ref="AM5:AM25" si="21">AD5*MAX($V5,AM$4)/$B$1</f>
-        <v>2475</v>
+        <v>198</v>
       </c>
       <c r="AN5">
         <f>MIN(AF5:AM5)</f>
@@ -2134,7 +2150,7 @@
       </c>
       <c r="E6" s="6">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>9</v>
@@ -2156,7 +2172,7 @@
       </c>
       <c r="V6">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="W6">
         <f t="shared" si="6"/>
@@ -2196,35 +2212,35 @@
       </c>
       <c r="AG6">
         <f t="shared" si="15"/>
-        <v>15.75</v>
+        <v>6.3</v>
       </c>
       <c r="AH6">
         <f t="shared" si="16"/>
-        <v>26.25</v>
+        <v>5.25</v>
       </c>
       <c r="AI6">
         <f t="shared" si="17"/>
-        <v>65.625</v>
+        <v>5.25</v>
       </c>
       <c r="AJ6">
         <f t="shared" si="18"/>
-        <v>131.25</v>
+        <v>10.5</v>
       </c>
       <c r="AK6">
         <f t="shared" si="19"/>
-        <v>184</v>
+        <v>14.72</v>
       </c>
       <c r="AL6">
         <f t="shared" si="20"/>
-        <v>761.25</v>
+        <v>60.9</v>
       </c>
       <c r="AM6">
         <f t="shared" si="21"/>
-        <v>1396.5</v>
+        <v>111.72</v>
       </c>
       <c r="AN6">
         <f t="shared" ref="AN6:AN24" si="22">MIN(AF6:AM6)</f>
-        <v>6.3</v>
+        <v>5.25</v>
       </c>
     </row>
     <row r="7" spans="1:40" x14ac:dyDescent="0.25">
@@ -2242,7 +2258,7 @@
       </c>
       <c r="E7" s="6">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>18</v>
@@ -2268,7 +2284,7 @@
       <c r="R7" s="1"/>
       <c r="V7">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="W7">
         <f t="shared" si="6"/>
@@ -2308,35 +2324,35 @@
       </c>
       <c r="AG7">
         <f t="shared" si="15"/>
-        <v>3.4250000000000003</v>
+        <v>1.37</v>
       </c>
       <c r="AH7">
         <f t="shared" si="16"/>
-        <v>6.25</v>
+        <v>1.25</v>
       </c>
       <c r="AI7">
         <f t="shared" si="17"/>
-        <v>21.125</v>
+        <v>1.69</v>
       </c>
       <c r="AJ7">
         <f t="shared" si="18"/>
-        <v>28.000000000000004</v>
+        <v>2.2400000000000002</v>
       </c>
       <c r="AK7">
         <f t="shared" si="19"/>
-        <v>53.349999999999994</v>
+        <v>4.2679999999999998</v>
       </c>
       <c r="AL7">
         <f t="shared" si="20"/>
-        <v>222.34</v>
+        <v>17.787199999999999</v>
       </c>
       <c r="AM7">
         <f t="shared" si="21"/>
-        <v>444.68</v>
+        <v>35.574399999999997</v>
       </c>
       <c r="AN7">
         <f t="shared" si="22"/>
-        <v>1.37</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="8" spans="1:40" x14ac:dyDescent="0.25">
@@ -2354,7 +2370,7 @@
       </c>
       <c r="E8" s="6">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>13</v>
@@ -2379,7 +2395,7 @@
       </c>
       <c r="V8">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="W8">
         <f t="shared" si="6"/>
@@ -2419,35 +2435,35 @@
       </c>
       <c r="AG8">
         <f t="shared" si="15"/>
-        <v>18.350000000000001</v>
+        <v>7.34</v>
       </c>
       <c r="AH8">
         <f t="shared" si="16"/>
-        <v>33.15</v>
+        <v>6.63</v>
       </c>
       <c r="AI8">
         <f t="shared" si="17"/>
-        <v>79.25</v>
+        <v>6.34</v>
       </c>
       <c r="AJ8">
         <f t="shared" si="18"/>
-        <v>158.5</v>
+        <v>12.68</v>
       </c>
       <c r="AK8">
         <f t="shared" si="19"/>
-        <v>274.5</v>
+        <v>21.96</v>
       </c>
       <c r="AL8">
         <f t="shared" si="20"/>
-        <v>1195.6299999999999</v>
+        <v>95.650399999999991</v>
       </c>
       <c r="AM8">
         <f t="shared" si="21"/>
-        <v>2082.7149999999997</v>
+        <v>166.61719999999997</v>
       </c>
       <c r="AN8">
         <f t="shared" si="22"/>
-        <v>7.34</v>
+        <v>6.34</v>
       </c>
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.25">
@@ -2465,7 +2481,7 @@
       </c>
       <c r="E9" s="6">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>17</v>
@@ -2481,7 +2497,7 @@
       </c>
       <c r="V9">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="W9">
         <f t="shared" si="6"/>
@@ -2521,35 +2537,35 @@
       </c>
       <c r="AG9">
         <f t="shared" si="15"/>
-        <v>8.2999999999999989</v>
+        <v>3.32</v>
       </c>
       <c r="AH9">
         <f t="shared" si="16"/>
-        <v>16.599999999999998</v>
+        <v>3.32</v>
       </c>
       <c r="AI9">
         <f t="shared" si="17"/>
-        <v>37.75</v>
+        <v>3.02</v>
       </c>
       <c r="AJ9">
         <f t="shared" si="18"/>
-        <v>75.5</v>
+        <v>6.04</v>
       </c>
       <c r="AK9">
         <f t="shared" si="19"/>
-        <v>136.5</v>
+        <v>10.92</v>
       </c>
       <c r="AL9">
         <f t="shared" si="20"/>
-        <v>682.5</v>
+        <v>54.6</v>
       </c>
       <c r="AM9">
         <f t="shared" si="21"/>
-        <v>1365</v>
+        <v>109.2</v>
       </c>
       <c r="AN9">
         <f t="shared" si="22"/>
-        <v>3.32</v>
+        <v>3.02</v>
       </c>
     </row>
     <row r="10" spans="1:40" x14ac:dyDescent="0.25">
@@ -2567,7 +2583,7 @@
       </c>
       <c r="E10" s="6">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>22</v>
@@ -2586,7 +2602,7 @@
       </c>
       <c r="V10">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="W10">
         <f t="shared" si="6"/>
@@ -2626,35 +2642,35 @@
       </c>
       <c r="AG10">
         <f t="shared" si="15"/>
-        <v>8.2750000000000004</v>
+        <v>3.31</v>
       </c>
       <c r="AH10">
         <f t="shared" si="16"/>
-        <v>14.9</v>
+        <v>2.98</v>
       </c>
       <c r="AI10">
         <f t="shared" si="17"/>
-        <v>35.125</v>
+        <v>2.81</v>
       </c>
       <c r="AJ10">
         <f t="shared" si="18"/>
-        <v>70.25</v>
+        <v>5.62</v>
       </c>
       <c r="AK10">
         <f t="shared" si="19"/>
-        <v>115.5</v>
+        <v>9.24</v>
       </c>
       <c r="AL10">
         <f t="shared" si="20"/>
-        <v>577.5</v>
+        <v>46.2</v>
       </c>
       <c r="AM10">
         <f t="shared" si="21"/>
-        <v>1155</v>
+        <v>92.4</v>
       </c>
       <c r="AN10">
         <f t="shared" si="22"/>
-        <v>3.31</v>
+        <v>2.81</v>
       </c>
     </row>
     <row r="11" spans="1:40" x14ac:dyDescent="0.25">
@@ -2672,7 +2688,7 @@
       </c>
       <c r="E11" s="6">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>88</v>
@@ -2691,7 +2707,7 @@
       </c>
       <c r="V11">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="W11">
         <f t="shared" si="6"/>
@@ -2731,35 +2747,35 @@
       </c>
       <c r="AG11">
         <f t="shared" si="15"/>
-        <v>0.44999999999999996</v>
+        <v>0.36</v>
       </c>
       <c r="AH11">
         <f t="shared" si="16"/>
-        <v>0.65</v>
+        <v>0.26</v>
       </c>
       <c r="AI11">
         <f t="shared" si="17"/>
-        <v>1.625</v>
+        <v>0.26</v>
       </c>
       <c r="AJ11">
         <f t="shared" si="18"/>
-        <v>3.25</v>
+        <v>0.26</v>
       </c>
       <c r="AK11">
         <f t="shared" si="19"/>
-        <v>3.0550000000000002</v>
+        <v>0.24440000000000001</v>
       </c>
       <c r="AL11">
         <f t="shared" si="20"/>
-        <v>15.275</v>
+        <v>1.222</v>
       </c>
       <c r="AM11">
         <f t="shared" si="21"/>
-        <v>17.72</v>
+        <v>1.4176</v>
       </c>
       <c r="AN11">
         <f t="shared" si="22"/>
-        <v>0.36</v>
+        <v>0.24440000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.25">
@@ -2777,7 +2793,7 @@
       </c>
       <c r="E12" s="6">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>95</v>
@@ -2799,7 +2815,7 @@
       </c>
       <c r="V12">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="W12">
         <f t="shared" si="6"/>
@@ -2839,35 +2855,35 @@
       </c>
       <c r="AG12">
         <f t="shared" si="15"/>
-        <v>1.6</v>
+        <v>0.64</v>
       </c>
       <c r="AH12">
         <f t="shared" si="16"/>
-        <v>2.2650000000000001</v>
+        <v>0.45300000000000007</v>
       </c>
       <c r="AI12">
         <f t="shared" si="17"/>
-        <v>5.6625000000000005</v>
+        <v>0.45300000000000007</v>
       </c>
       <c r="AJ12">
         <f t="shared" si="18"/>
-        <v>11.325000000000001</v>
+        <v>0.90600000000000014</v>
       </c>
       <c r="AK12">
         <f t="shared" si="19"/>
-        <v>14.899999999999999</v>
+        <v>1.1919999999999999</v>
       </c>
       <c r="AL12">
         <f t="shared" si="20"/>
-        <v>55.190000000000005</v>
+        <v>4.4152000000000005</v>
       </c>
       <c r="AM12">
         <f t="shared" si="21"/>
-        <v>93.820000000000007</v>
+        <v>7.5056000000000003</v>
       </c>
       <c r="AN12">
         <f t="shared" ref="AN12" si="23">MIN(AF12:AM12)</f>
-        <v>0.64</v>
+        <v>0.45300000000000007</v>
       </c>
     </row>
     <row r="13" spans="1:40" x14ac:dyDescent="0.25">
@@ -2885,7 +2901,7 @@
       </c>
       <c r="E13" s="6">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>94</v>
@@ -2907,7 +2923,7 @@
       </c>
       <c r="V13">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="W13">
         <f t="shared" ref="W13" si="24">K13</f>
@@ -2947,35 +2963,35 @@
       </c>
       <c r="AG13">
         <f t="shared" ref="AG13" si="33">X13*MAX($V13,AG$4)/$B$1</f>
-        <v>1.1500000000000001</v>
+        <v>0.92</v>
       </c>
       <c r="AH13">
         <f t="shared" ref="AH13" si="34">Y13*MAX($V13,AH$4)/$B$1</f>
-        <v>1.61</v>
+        <v>0.64400000000000002</v>
       </c>
       <c r="AI13">
         <f t="shared" ref="AI13" si="35">Z13*MAX($V13,AI$4)/$B$1</f>
-        <v>4.0250000000000004</v>
+        <v>0.64400000000000002</v>
       </c>
       <c r="AJ13">
         <f t="shared" ref="AJ13" si="36">AA13*MAX($V13,AJ$4)/$B$1</f>
-        <v>8.0500000000000007</v>
+        <v>0.64400000000000002</v>
       </c>
       <c r="AK13">
         <f t="shared" ref="AK13" si="37">AB13*MAX($V13,AK$4)/$B$1</f>
-        <v>9.65</v>
+        <v>0.77200000000000002</v>
       </c>
       <c r="AL13">
         <f t="shared" ref="AL13" si="38">AC13*MAX($V13,AL$4)/$B$1</f>
-        <v>36.19</v>
+        <v>2.8952</v>
       </c>
       <c r="AM13">
         <f t="shared" ref="AM13" si="39">AD13*MAX($V13,AM$4)/$B$1</f>
-        <v>61.12</v>
+        <v>4.8895999999999997</v>
       </c>
       <c r="AN13">
         <f t="shared" ref="AN13" si="40">MIN(AF13:AM13)</f>
-        <v>0.92</v>
+        <v>0.64400000000000002</v>
       </c>
     </row>
     <row r="14" spans="1:40" x14ac:dyDescent="0.25">
@@ -2993,7 +3009,7 @@
       </c>
       <c r="E14" s="6">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>49</v>
@@ -3015,7 +3031,7 @@
       </c>
       <c r="V14">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="W14">
         <f t="shared" si="6"/>
@@ -3055,35 +3071,35 @@
       </c>
       <c r="AG14">
         <f t="shared" si="15"/>
-        <v>0.44999999999999996</v>
+        <v>0.18</v>
       </c>
       <c r="AH14">
         <f t="shared" si="16"/>
-        <v>0.60499999999999998</v>
+        <v>0.121</v>
       </c>
       <c r="AI14">
         <f t="shared" si="17"/>
-        <v>1.5125</v>
+        <v>0.121</v>
       </c>
       <c r="AJ14">
         <f t="shared" si="18"/>
-        <v>3.0249999999999999</v>
+        <v>0.24199999999999999</v>
       </c>
       <c r="AK14">
         <f t="shared" si="19"/>
-        <v>3.05</v>
+        <v>0.24399999999999999</v>
       </c>
       <c r="AL14">
         <f t="shared" si="20"/>
-        <v>10.51</v>
+        <v>0.84079999999999999</v>
       </c>
       <c r="AM14">
         <f t="shared" si="21"/>
-        <v>18.594999999999999</v>
+        <v>1.4875999999999998</v>
       </c>
       <c r="AN14">
         <f t="shared" si="22"/>
-        <v>0.18</v>
+        <v>0.121</v>
       </c>
     </row>
     <row r="15" spans="1:40" x14ac:dyDescent="0.25">
@@ -3101,7 +3117,7 @@
       </c>
       <c r="E15" s="6">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>96</v>
@@ -3123,7 +3139,7 @@
       </c>
       <c r="V15">
         <f t="shared" si="5"/>
-        <v>8</v>
+        <v>100</v>
       </c>
       <c r="W15">
         <f t="shared" si="6"/>
@@ -3167,31 +3183,31 @@
       </c>
       <c r="AH15">
         <f t="shared" si="16"/>
-        <v>0.41500000000000004</v>
+        <v>0.33200000000000002</v>
       </c>
       <c r="AI15">
         <f t="shared" si="17"/>
-        <v>1.0375000000000001</v>
+        <v>0.33200000000000002</v>
       </c>
       <c r="AJ15">
         <f t="shared" si="18"/>
-        <v>2.0750000000000002</v>
+        <v>0.33200000000000002</v>
       </c>
       <c r="AK15">
         <f t="shared" si="19"/>
-        <v>1.8599999999999999</v>
+        <v>0.14879999999999999</v>
       </c>
       <c r="AL15">
         <f t="shared" si="20"/>
-        <v>6.64</v>
+        <v>0.53120000000000001</v>
       </c>
       <c r="AM15">
         <f t="shared" si="21"/>
-        <v>10.435</v>
+        <v>0.83479999999999999</v>
       </c>
       <c r="AN15">
         <f t="shared" si="22"/>
-        <v>0.41500000000000004</v>
+        <v>0.14879999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:40" x14ac:dyDescent="0.25">
@@ -3209,7 +3225,7 @@
       </c>
       <c r="E16" s="6">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>50</v>
@@ -3231,7 +3247,7 @@
       </c>
       <c r="V16">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="W16">
         <f t="shared" si="6"/>
@@ -3271,35 +3287,35 @@
       </c>
       <c r="AG16">
         <f t="shared" si="15"/>
-        <v>0.35000000000000003</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="AH16">
         <f t="shared" si="16"/>
-        <v>0.65</v>
+        <v>0.13</v>
       </c>
       <c r="AI16">
         <f t="shared" si="17"/>
-        <v>1.625</v>
+        <v>0.13</v>
       </c>
       <c r="AJ16">
         <f t="shared" si="18"/>
-        <v>3.25</v>
+        <v>0.26</v>
       </c>
       <c r="AK16">
         <f t="shared" si="19"/>
-        <v>4.3</v>
+        <v>0.34399999999999997</v>
       </c>
       <c r="AL16">
         <f t="shared" si="20"/>
-        <v>17.97</v>
+        <v>1.4376</v>
       </c>
       <c r="AM16">
         <f t="shared" si="21"/>
-        <v>30.19</v>
+        <v>2.4152</v>
       </c>
       <c r="AN16">
         <f t="shared" si="22"/>
-        <v>0.14000000000000001</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="17" spans="1:40" x14ac:dyDescent="0.25">
@@ -3317,7 +3333,7 @@
       </c>
       <c r="E17" s="6">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>90</v>
@@ -3336,7 +3352,7 @@
       </c>
       <c r="V17">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>125</v>
       </c>
       <c r="W17">
         <f t="shared" si="6"/>
@@ -3384,27 +3400,27 @@
       </c>
       <c r="AI17">
         <f t="shared" si="17"/>
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="AJ17">
         <f t="shared" si="18"/>
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="AK17">
         <f t="shared" si="19"/>
-        <v>0.81499999999999995</v>
+        <v>8.1499999999999989E-2</v>
       </c>
       <c r="AL17">
         <f t="shared" si="20"/>
-        <v>4.0749999999999993</v>
+        <v>0.32599999999999996</v>
       </c>
       <c r="AM17">
         <f t="shared" si="21"/>
-        <v>3.6549999999999998</v>
+        <v>0.29239999999999999</v>
       </c>
       <c r="AN17">
         <f t="shared" si="22"/>
-        <v>0.2</v>
+        <v>8.1499999999999989E-2</v>
       </c>
     </row>
     <row r="18" spans="1:40" x14ac:dyDescent="0.25">
@@ -3422,7 +3438,7 @@
       </c>
       <c r="E18" s="6">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>91</v>
@@ -3441,7 +3457,7 @@
       </c>
       <c r="V18">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="W18">
         <f t="shared" si="6"/>
@@ -3481,35 +3497,35 @@
       </c>
       <c r="AG18">
         <f t="shared" si="15"/>
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="AH18">
         <f t="shared" si="16"/>
-        <v>0.2</v>
+        <v>0.08</v>
       </c>
       <c r="AI18">
         <f t="shared" si="17"/>
-        <v>0.5</v>
+        <v>0.08</v>
       </c>
       <c r="AJ18">
         <f t="shared" si="18"/>
-        <v>1</v>
+        <v>0.08</v>
       </c>
       <c r="AK18">
         <f t="shared" si="19"/>
-        <v>0.81499999999999995</v>
+        <v>6.5199999999999994E-2</v>
       </c>
       <c r="AL18">
         <f t="shared" si="20"/>
-        <v>4.0749999999999993</v>
+        <v>0.32599999999999996</v>
       </c>
       <c r="AM18">
         <f t="shared" si="21"/>
-        <v>3.6549999999999998</v>
+        <v>0.29239999999999999</v>
       </c>
       <c r="AN18">
         <f t="shared" si="22"/>
-        <v>0.2</v>
+        <v>6.5199999999999994E-2</v>
       </c>
     </row>
     <row r="19" spans="1:40" x14ac:dyDescent="0.25">
@@ -3527,7 +3543,7 @@
       </c>
       <c r="E19" s="6">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>86</v>
@@ -3558,7 +3574,7 @@
       </c>
       <c r="V19">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="W19">
         <f t="shared" si="6"/>
@@ -3598,41 +3614,44 @@
       </c>
       <c r="AG19">
         <f t="shared" si="15"/>
-        <v>2.27</v>
+        <v>0.90799999999999992</v>
       </c>
       <c r="AH19">
         <f t="shared" si="16"/>
-        <v>3.95</v>
+        <v>0.79</v>
       </c>
       <c r="AI19">
         <f t="shared" si="17"/>
-        <v>8.68</v>
+        <v>0.69440000000000002</v>
       </c>
       <c r="AJ19">
         <f t="shared" si="18"/>
-        <v>14.42</v>
+        <v>1.1536</v>
       </c>
       <c r="AK19">
         <f t="shared" si="19"/>
-        <v>24.565000000000001</v>
+        <v>1.9652000000000001</v>
       </c>
       <c r="AL19">
         <f t="shared" si="20"/>
-        <v>106.80000000000001</v>
+        <v>8.5440000000000005</v>
       </c>
       <c r="AM19">
         <f t="shared" si="21"/>
-        <v>186.9</v>
+        <v>14.952</v>
       </c>
       <c r="AN19">
         <f t="shared" si="22"/>
-        <v>0.95</v>
+        <v>0.69440000000000002</v>
       </c>
     </row>
     <row r="20" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>59</v>
       </c>
+      <c r="B20" t="s">
+        <v>98</v>
+      </c>
       <c r="C20" t="s">
         <v>85</v>
       </c>
@@ -3641,7 +3660,7 @@
       </c>
       <c r="E20" s="6">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>58</v>
@@ -3663,7 +3682,7 @@
       </c>
       <c r="V20">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="W20">
         <f t="shared" ref="W20" si="41">K20</f>
@@ -3703,35 +3722,35 @@
       </c>
       <c r="AG20">
         <f t="shared" ref="AG20" si="50">X20*MAX($V20,AG$4)/$B$1</f>
-        <v>1.2250000000000001</v>
+        <v>0.49</v>
       </c>
       <c r="AH20">
         <f t="shared" ref="AH20" si="51">Y20*MAX($V20,AH$4)/$B$1</f>
-        <v>1.7799999999999998</v>
+        <v>0.35600000000000004</v>
       </c>
       <c r="AI20">
         <f t="shared" ref="AI20" si="52">Z20*MAX($V20,AI$4)/$B$1</f>
-        <v>4.45</v>
+        <v>0.35600000000000004</v>
       </c>
       <c r="AJ20">
         <f t="shared" ref="AJ20" si="53">AA20*MAX($V20,AJ$4)/$B$1</f>
-        <v>8.9</v>
+        <v>0.71200000000000008</v>
       </c>
       <c r="AK20">
         <f t="shared" ref="AK20" si="54">AB20*MAX($V20,AK$4)/$B$1</f>
-        <v>11.600000000000001</v>
+        <v>0.92800000000000016</v>
       </c>
       <c r="AL20">
         <f t="shared" ref="AL20" si="55">AC20*MAX($V20,AL$4)/$B$1</f>
-        <v>41.72</v>
+        <v>3.3376000000000001</v>
       </c>
       <c r="AM20">
         <f t="shared" ref="AM20" si="56">AD20*MAX($V20,AM$4)/$B$1</f>
-        <v>65.305000000000007</v>
+        <v>5.2244000000000002</v>
       </c>
       <c r="AN20">
         <f t="shared" ref="AN20" si="57">MIN(AF20:AM20)</f>
-        <v>0.49</v>
+        <v>0.35600000000000004</v>
       </c>
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.25">
@@ -3746,7 +3765,7 @@
       </c>
       <c r="E21" s="6">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>31</v>
@@ -3775,7 +3794,7 @@
       </c>
       <c r="V21">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="W21">
         <f t="shared" si="6"/>
@@ -3815,35 +3834,35 @@
       </c>
       <c r="AG21">
         <f t="shared" si="15"/>
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="AH21">
         <f t="shared" si="16"/>
-        <v>3.5</v>
+        <v>0.7</v>
       </c>
       <c r="AI21">
         <f t="shared" si="17"/>
-        <v>4</v>
+        <v>0.32</v>
       </c>
       <c r="AJ21">
         <f t="shared" si="18"/>
-        <v>7.0000000000000009</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="AK21">
         <f t="shared" si="19"/>
-        <v>8.5</v>
+        <v>0.68</v>
       </c>
       <c r="AL21">
         <f t="shared" si="20"/>
-        <v>42.5</v>
+        <v>3.4</v>
       </c>
       <c r="AM21">
         <f t="shared" si="21"/>
-        <v>85</v>
+        <v>6.8</v>
       </c>
       <c r="AN21">
         <f t="shared" si="22"/>
-        <v>2.5</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="22" spans="1:40" x14ac:dyDescent="0.25">
@@ -3858,7 +3877,7 @@
       </c>
       <c r="E22" s="6">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>30</v>
@@ -3889,7 +3908,7 @@
       </c>
       <c r="V22">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="W22">
         <f t="shared" si="6"/>
@@ -3929,35 +3948,35 @@
       </c>
       <c r="AG22">
         <f t="shared" si="15"/>
-        <v>44.155000000000001</v>
+        <v>17.661999999999999</v>
       </c>
       <c r="AH22">
         <f t="shared" si="16"/>
-        <v>46.69</v>
+        <v>9.3379999999999992</v>
       </c>
       <c r="AI22">
         <f t="shared" si="17"/>
-        <v>50.68</v>
+        <v>4.0544000000000002</v>
       </c>
       <c r="AJ22">
         <f t="shared" si="18"/>
-        <v>78.180000000000007</v>
+        <v>6.2544000000000004</v>
       </c>
       <c r="AK22">
         <f t="shared" si="19"/>
-        <v>126</v>
+        <v>10.08</v>
       </c>
       <c r="AL22">
         <f t="shared" si="20"/>
-        <v>630</v>
+        <v>50.4</v>
       </c>
       <c r="AM22">
         <f t="shared" si="21"/>
-        <v>1260</v>
+        <v>100.8</v>
       </c>
       <c r="AN22">
         <f t="shared" si="22"/>
-        <v>44.155000000000001</v>
+        <v>4.0544000000000002</v>
       </c>
     </row>
     <row r="23" spans="1:40" x14ac:dyDescent="0.25">
@@ -3972,7 +3991,7 @@
       </c>
       <c r="E23" s="6">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>39</v>
@@ -3990,7 +4009,7 @@
       </c>
       <c r="V23">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="W23">
         <f t="shared" si="6"/>
@@ -4030,35 +4049,35 @@
       </c>
       <c r="AG23">
         <f t="shared" si="15"/>
-        <v>17.855</v>
+        <v>7.1420000000000003</v>
       </c>
       <c r="AH23">
         <f t="shared" si="16"/>
-        <v>17.855</v>
+        <v>3.5710000000000002</v>
       </c>
       <c r="AI23">
         <f t="shared" si="17"/>
-        <v>44.637500000000003</v>
+        <v>3.5710000000000002</v>
       </c>
       <c r="AJ23">
         <f t="shared" si="18"/>
-        <v>89.275000000000006</v>
+        <v>7.1420000000000003</v>
       </c>
       <c r="AK23">
         <f t="shared" si="19"/>
-        <v>178.55</v>
+        <v>14.284000000000001</v>
       </c>
       <c r="AL23">
         <f t="shared" si="20"/>
-        <v>892.75</v>
+        <v>71.42</v>
       </c>
       <c r="AM23">
         <f t="shared" si="21"/>
-        <v>1785.5</v>
+        <v>142.84</v>
       </c>
       <c r="AN23">
         <f t="shared" si="22"/>
-        <v>17.855</v>
+        <v>3.5710000000000002</v>
       </c>
     </row>
     <row r="24" spans="1:40" x14ac:dyDescent="0.25">
@@ -4073,7 +4092,7 @@
       </c>
       <c r="E24" s="6">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>44</v>
@@ -4095,7 +4114,7 @@
       </c>
       <c r="V24">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="W24">
         <f t="shared" si="6"/>
@@ -4135,35 +4154,35 @@
       </c>
       <c r="AG24">
         <f t="shared" si="15"/>
-        <v>7.17</v>
+        <v>2.8680000000000003</v>
       </c>
       <c r="AH24">
         <f t="shared" si="16"/>
-        <v>7.93</v>
+        <v>1.5859999999999999</v>
       </c>
       <c r="AI24">
         <f t="shared" si="17"/>
-        <v>19.824999999999999</v>
+        <v>1.5859999999999999</v>
       </c>
       <c r="AJ24">
         <f t="shared" si="18"/>
-        <v>39.65</v>
+        <v>3.1719999999999997</v>
       </c>
       <c r="AK24">
         <f t="shared" si="19"/>
-        <v>79.3</v>
+        <v>6.3439999999999994</v>
       </c>
       <c r="AL24">
         <f t="shared" si="20"/>
-        <v>396.49999999999994</v>
+        <v>31.719999999999995</v>
       </c>
       <c r="AM24">
         <f t="shared" si="21"/>
-        <v>792.99999999999989</v>
+        <v>63.439999999999991</v>
       </c>
       <c r="AN24">
         <f t="shared" si="22"/>
-        <v>7.17</v>
+        <v>1.5859999999999999</v>
       </c>
     </row>
     <row r="25" spans="1:40" x14ac:dyDescent="0.25">
@@ -4178,7 +4197,7 @@
       </c>
       <c r="E25" s="6">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>41</v>
@@ -4208,7 +4227,7 @@
       </c>
       <c r="V25">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="W25">
         <f t="shared" si="6"/>
@@ -4248,35 +4267,35 @@
       </c>
       <c r="AG25">
         <f t="shared" si="15"/>
-        <v>4.335</v>
+        <v>1.734</v>
       </c>
       <c r="AH25">
         <f t="shared" si="16"/>
-        <v>4.335</v>
+        <v>0.86699999999999999</v>
       </c>
       <c r="AI25">
         <f t="shared" si="17"/>
-        <v>8.67</v>
+        <v>0.69359999999999999</v>
       </c>
       <c r="AJ25">
         <f t="shared" si="18"/>
-        <v>21.675000000000001</v>
+        <v>1.734</v>
       </c>
       <c r="AK25">
         <f t="shared" si="19"/>
-        <v>43.35</v>
+        <v>3.468</v>
       </c>
       <c r="AL25">
         <f t="shared" si="20"/>
-        <v>216.75</v>
+        <v>17.34</v>
       </c>
       <c r="AM25">
         <f t="shared" si="21"/>
-        <v>433.5</v>
+        <v>34.68</v>
       </c>
       <c r="AN25">
         <f t="shared" ref="AN25" si="58">MIN(AF25:AM25)</f>
-        <v>4.335</v>
+        <v>0.69359999999999999</v>
       </c>
     </row>
     <row r="26" spans="1:40" x14ac:dyDescent="0.25">
@@ -4285,12 +4304,20 @@
       </c>
       <c r="AN26">
         <f>SUM(AN5:AN25)</f>
-        <v>107.1</v>
+        <v>36.783299999999997</v>
       </c>
     </row>
     <row r="27" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:40" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add 2*3 100 mil header to BOM
</commit_message>
<xml_diff>
--- a/pcb/draft_1-2/BOM.xlsx
+++ b/pcb/draft_1-2/BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\EletronicEgg\pcb\draft_1-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F313FFCC-8FF0-4509-8BFF-44091B770F0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A94F23E9-DE29-43C5-8DF7-E1AF246F619C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CC748F4A-B77A-42D3-919B-40EFF9144FCF}"/>
   </bookViews>
@@ -20,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
   <si>
     <t>400 mAh Battery</t>
   </si>
@@ -334,6 +328,12 @@
   </si>
   <si>
     <t>J2</t>
+  </si>
+  <si>
+    <t>2*3 100 mil header</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/PH2-06-UA/2057-PH2-06-UA-ND/9830396/?itemSeq=351205478</t>
   </si>
 </sst>
 </file>
@@ -526,7 +526,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>BOM!$Y$30:$Y$50</c:f>
+              <c:f>BOM!$Y$31:$Y$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -598,7 +598,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>BOM!$Z$30:$Z$50</c:f>
+              <c:f>BOM!$Z$31:$Z$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -1538,13 +1538,13 @@
     <xdr:from>
       <xdr:col>26</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>71437</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1870,10 +1870,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E8EB424-57BA-4A49-86A1-3A232E6B3ACD}">
-  <dimension ref="A1:AN50"/>
+  <dimension ref="A1:AN51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1912,7 +1912,7 @@
         <v>54</v>
       </c>
       <c r="B2" s="8">
-        <f>AN26</f>
+        <f>AN27</f>
         <v>36.783299999999997</v>
       </c>
       <c r="C2" s="8"/>
@@ -2063,7 +2063,7 @@
         <v>4.95</v>
       </c>
       <c r="V5">
-        <f t="shared" ref="V5:V25" si="5">B$1*D5</f>
+        <f t="shared" ref="V5:V26" si="5">B$1*D5</f>
         <v>25</v>
       </c>
       <c r="W5">
@@ -4300,228 +4300,244 @@
     </row>
     <row r="26" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>101</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="V26">
+        <f t="shared" si="5"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>56</v>
       </c>
-      <c r="AN26">
+      <c r="AN27">
         <f>SUM(AN5:AN25)</f>
         <v>36.783299999999997</v>
       </c>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B29" s="10" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="Y30">
-        <v>1</v>
-      </c>
-      <c r="Z30">
-        <v>180.82999999999998</v>
       </c>
     </row>
     <row r="31" spans="1:40" x14ac:dyDescent="0.25">
       <c r="Y31">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="Z31">
-        <v>58.201000000000008</v>
+        <v>180.82999999999998</v>
       </c>
     </row>
     <row r="32" spans="1:40" x14ac:dyDescent="0.25">
       <c r="Y32">
-        <f>Y31+5</f>
+        <v>5</v>
+      </c>
+      <c r="Z32">
+        <v>58.201000000000008</v>
+      </c>
+    </row>
+    <row r="33" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y33">
+        <f>Y32+5</f>
         <v>10</v>
       </c>
-      <c r="Z32">
+      <c r="Z33">
         <v>41.628499999999988</v>
       </c>
     </row>
-    <row r="33" spans="25:30" x14ac:dyDescent="0.25">
-      <c r="Y33">
-        <f t="shared" ref="Y33:Y50" si="59">Y32+5</f>
+    <row r="34" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y34">
+        <f t="shared" ref="Y34:Y51" si="59">Y33+5</f>
         <v>15</v>
       </c>
-      <c r="Z33">
+      <c r="Z34">
         <v>38.548333333333325</v>
       </c>
     </row>
-    <row r="34" spans="25:30" x14ac:dyDescent="0.25">
-      <c r="Y34">
+    <row r="35" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y35">
         <f t="shared" si="59"/>
         <v>20</v>
       </c>
-      <c r="Z34">
+      <c r="Z35">
         <v>36.639999999999993</v>
       </c>
     </row>
-    <row r="35" spans="25:30" x14ac:dyDescent="0.25">
-      <c r="Y35">
+    <row r="36" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y36">
         <f t="shared" si="59"/>
         <v>25</v>
       </c>
-      <c r="Z35">
+      <c r="Z36">
         <v>34.514600000000002</v>
       </c>
     </row>
-    <row r="36" spans="25:30" x14ac:dyDescent="0.25">
-      <c r="Y36">
+    <row r="37" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y37">
         <f t="shared" si="59"/>
         <v>30</v>
       </c>
-      <c r="Z36">
+      <c r="Z37">
         <v>34.448333333333323</v>
       </c>
     </row>
-    <row r="37" spans="25:30" x14ac:dyDescent="0.25">
-      <c r="Y37">
+    <row r="38" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y38">
         <f t="shared" si="59"/>
         <v>35</v>
       </c>
-      <c r="Z37">
+      <c r="Z38">
         <v>34.411285714285711</v>
       </c>
     </row>
-    <row r="38" spans="25:30" x14ac:dyDescent="0.25">
-      <c r="Y38">
+    <row r="39" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y39">
         <f t="shared" si="59"/>
         <v>40</v>
       </c>
-      <c r="Z38">
+      <c r="Z39">
         <v>34.246099999999998</v>
       </c>
     </row>
-    <row r="39" spans="25:30" x14ac:dyDescent="0.25">
-      <c r="Y39">
+    <row r="40" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y40">
         <f t="shared" si="59"/>
         <v>45</v>
       </c>
-      <c r="Z39">
+      <c r="Z40">
         <v>33.778599999999997</v>
       </c>
     </row>
-    <row r="40" spans="25:30" x14ac:dyDescent="0.25">
-      <c r="Y40">
+    <row r="41" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y41">
         <f t="shared" si="59"/>
         <v>50</v>
       </c>
-      <c r="Z40">
+      <c r="Z41">
         <v>33.260599999999997</v>
       </c>
     </row>
-    <row r="41" spans="25:30" x14ac:dyDescent="0.25">
-      <c r="Y41">
+    <row r="42" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y42">
         <f t="shared" si="59"/>
         <v>55</v>
       </c>
-      <c r="Z41">
+      <c r="Z42">
         <v>33.260599999999997</v>
       </c>
     </row>
-    <row r="42" spans="25:30" x14ac:dyDescent="0.25">
-      <c r="Y42">
+    <row r="43" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y43">
         <f t="shared" si="59"/>
         <v>60</v>
       </c>
-      <c r="Z42">
+      <c r="Z43">
         <v>33.260599999999997</v>
       </c>
     </row>
-    <row r="43" spans="25:30" x14ac:dyDescent="0.25">
-      <c r="Y43">
+    <row r="44" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y44">
         <f t="shared" si="59"/>
         <v>65</v>
       </c>
-      <c r="Z43">
+      <c r="Z44">
         <v>33.24213846153846</v>
       </c>
     </row>
-    <row r="44" spans="25:30" x14ac:dyDescent="0.25">
-      <c r="Y44">
+    <row r="45" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y45">
         <f t="shared" si="59"/>
         <v>70</v>
       </c>
-      <c r="Z44">
+      <c r="Z45">
         <v>33.21631428571429</v>
       </c>
     </row>
-    <row r="45" spans="25:30" x14ac:dyDescent="0.25">
-      <c r="Y45">
+    <row r="46" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y46">
         <f t="shared" si="59"/>
         <v>75</v>
       </c>
-      <c r="Z45">
+      <c r="Z46">
         <v>32.84859999999999</v>
       </c>
     </row>
-    <row r="46" spans="25:30" x14ac:dyDescent="0.25">
-      <c r="Y46">
+    <row r="47" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y47">
         <f t="shared" si="59"/>
         <v>80</v>
       </c>
-      <c r="Z46">
+      <c r="Z47">
         <v>32.520600000000002</v>
       </c>
     </row>
-    <row r="47" spans="25:30" x14ac:dyDescent="0.25">
-      <c r="Y47">
+    <row r="48" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y48">
         <f t="shared" si="59"/>
         <v>85</v>
       </c>
-      <c r="Z47">
+      <c r="Z48">
         <v>31.976341176470587</v>
-      </c>
-    </row>
-    <row r="48" spans="25:30" x14ac:dyDescent="0.25">
-      <c r="Y48">
-        <f t="shared" si="59"/>
-        <v>90</v>
-      </c>
-      <c r="Z48">
-        <v>31.163400000000003</v>
-      </c>
-      <c r="AC48">
-        <v>10</v>
-      </c>
-      <c r="AD48" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="49" spans="25:30" x14ac:dyDescent="0.25">
       <c r="Y49">
         <f t="shared" si="59"/>
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="Z49">
-        <v>30.18182105263158</v>
+        <v>31.163400000000003</v>
       </c>
       <c r="AC49">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="AD49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="50" spans="25:30" x14ac:dyDescent="0.25">
       <c r="Y50">
         <f t="shared" si="59"/>
+        <v>95</v>
+      </c>
+      <c r="Z50">
+        <v>30.18182105263158</v>
+      </c>
+      <c r="AC50">
+        <v>25</v>
+      </c>
+      <c r="AD50" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" spans="25:30" x14ac:dyDescent="0.25">
+      <c r="Y51">
+        <f t="shared" si="59"/>
         <v>100</v>
       </c>
-      <c r="Z50">
+      <c r="Z51">
         <v>29.229300000000002</v>
       </c>
-      <c r="AC50">
+      <c r="AC51">
         <v>100</v>
       </c>
-      <c r="AD50" t="s">
+      <c r="AD51" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>